<commit_message>
progess work still working
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="50">
   <si>
     <t>employeeid</t>
   </si>
@@ -146,6 +146,21 @@
   </si>
   <si>
     <t>kk26@gmail.com</t>
+  </si>
+  <si>
+    <t>Monika</t>
+  </si>
+  <si>
+    <t>Mgonila26@gmail.com</t>
+  </si>
+  <si>
+    <t>backend</t>
+  </si>
+  <si>
+    <t>shreyansh</t>
+  </si>
+  <si>
+    <t>sj26@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -523,7 +538,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K12"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -885,6 +900,76 @@
         <v>9140834289</v>
       </c>
     </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1017</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="1">
+        <v>44485.44639960648</v>
+      </c>
+      <c r="K11">
+        <v>9140834289</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1018</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="1">
+        <v>44486.421475219904</v>
+      </c>
+      <c r="K12">
+        <v>9140834289</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
testing cloud update remain & design ,testing done
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>employeeid</t>
   </si>
@@ -46,19 +46,19 @@
     <t>phone</t>
   </si>
   <si>
-    <t>Shreya Jaiswal</t>
-  </si>
-  <si>
-    <t>minishreya221996@gmail.com</t>
-  </si>
-  <si>
-    <t>software</t>
-  </si>
-  <si>
-    <t>http://res.cloudinary.com/db5vn6bj5/image/upload/v1631979713/pdakv5si8r3yiukxa5ht.jpg</t>
-  </si>
-  <si>
-    <t>fresher</t>
+    <t>shreya Jaiswal</t>
+  </si>
+  <si>
+    <t>shreyajaiswalvns1996@gmail.com</t>
+  </si>
+  <si>
+    <t>backend</t>
+  </si>
+  <si>
+    <t>http://res.cloudinary.com/db5vn6bj5/image/upload/v1634903961/rfmurbjifwkiy1xh7jnc.jpg</t>
+  </si>
+  <si>
+    <t>Fresher</t>
   </si>
   <si>
     <t>delhi</t>
@@ -70,97 +70,16 @@
     <t>full time</t>
   </si>
   <si>
-    <t xml:space="preserve">kiran </t>
-  </si>
-  <si>
-    <t>mini@gmail.com</t>
-  </si>
-  <si>
-    <t>mumbai</t>
-  </si>
-  <si>
-    <t>chhaya</t>
-  </si>
-  <si>
-    <t>chhya@gmail.com</t>
-  </si>
-  <si>
-    <t>manager</t>
-  </si>
-  <si>
-    <t>manging client</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> shikhar Jaiswal</t>
-  </si>
-  <si>
-    <t>minishreya226@gmail.com</t>
-  </si>
-  <si>
-    <t>kk jain</t>
-  </si>
-  <si>
-    <t>m226@gmail.com</t>
-  </si>
-  <si>
-    <t>management</t>
-  </si>
-  <si>
-    <t>experience</t>
-  </si>
-  <si>
-    <t>Shreyansh Jaiswal</t>
-  </si>
-  <si>
-    <t>ss@gmail.com</t>
-  </si>
-  <si>
-    <t>analist</t>
-  </si>
-  <si>
-    <t>solution provider</t>
-  </si>
-  <si>
-    <t>BSC</t>
-  </si>
-  <si>
-    <t>contractor</t>
-  </si>
-  <si>
-    <t>M Khan</t>
-  </si>
-  <si>
-    <t>m256@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Senior software </t>
-  </si>
-  <si>
-    <t>shreya Jaiswal</t>
-  </si>
-  <si>
-    <t>jaiswal@gmail.com</t>
-  </si>
-  <si>
-    <t>Amir Khan</t>
-  </si>
-  <si>
-    <t>kk26@gmail.com</t>
-  </si>
-  <si>
-    <t>Monika</t>
-  </si>
-  <si>
-    <t>Mgonila26@gmail.com</t>
-  </si>
-  <si>
-    <t>backend</t>
-  </si>
-  <si>
-    <t>shreyansh</t>
-  </si>
-  <si>
-    <t>sj26@gmail.com</t>
+    <t>Abhishek gupta</t>
+  </si>
+  <si>
+    <t>iam.abhishekgupta01@gmail.com</t>
+  </si>
+  <si>
+    <t>Kajol</t>
+  </si>
+  <si>
+    <t>shreyajaiswal1996vns@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -538,7 +457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -587,7 +506,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1001</v>
+        <v>10000</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -614,7 +533,7 @@
         <v>18</v>
       </c>
       <c r="J2" s="1">
-        <v>44457.65392936343</v>
+        <v>44491.54326440972</v>
       </c>
       <c r="K2">
         <v>9140834289</v>
@@ -622,7 +541,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -640,7 +559,7 @@
         <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
         <v>17</v>
@@ -649,33 +568,33 @@
         <v>18</v>
       </c>
       <c r="J3" s="1">
-        <v>44457.65392936343</v>
+        <v>44491.54326440972</v>
       </c>
       <c r="K3">
-        <v>9140830000</v>
+        <v>8830073205</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
         <v>17</v>
@@ -684,289 +603,9 @@
         <v>18</v>
       </c>
       <c r="J4" s="1">
-        <v>44457.65392936343</v>
+        <v>44492.70294284722</v>
       </c>
       <c r="K4">
-        <v>9140830000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1004</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="1">
-        <v>44458.65577915509</v>
-      </c>
-      <c r="K5">
-        <v>9140834289</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1006</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="1">
-        <v>44458.665778229166</v>
-      </c>
-      <c r="K6">
-        <v>9140834289</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1007</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="1">
-        <v>44458.67840596064</v>
-      </c>
-      <c r="K7">
-        <v>9100830000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1008</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="1">
-        <v>44458.68801288195</v>
-      </c>
-      <c r="K8">
-        <v>9140834289</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1009</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" t="s">
-        <v>37</v>
-      </c>
-      <c r="J9" s="1">
-        <v>44459.264242060184</v>
-      </c>
-      <c r="K9">
-        <v>9100830001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1012</v>
-      </c>
-      <c r="B10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="1">
-        <v>44460.27493564815</v>
-      </c>
-      <c r="K10">
-        <v>9140834289</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1017</v>
-      </c>
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="1">
-        <v>44485.44639960648</v>
-      </c>
-      <c r="K11">
-        <v>9140834289</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1018</v>
-      </c>
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="1">
-        <v>44486.421475219904</v>
-      </c>
-      <c r="K12">
         <v>9140834289</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified and test update
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t>employeeid</t>
   </si>
@@ -76,10 +76,76 @@
     <t>iam.abhishekgupta01@gmail.com</t>
   </si>
   <si>
+    <t>fynd Accedamy</t>
+  </si>
+  <si>
+    <t>http://res.cloudinary.com/db5vn6bj5/image/upload/v1635076447/durz7fokpsouywmymjib.jpg</t>
+  </si>
+  <si>
+    <t>Experiance</t>
+  </si>
+  <si>
+    <t>Navi mumbai</t>
+  </si>
+  <si>
+    <t>BSC</t>
+  </si>
+  <si>
     <t>Kajol</t>
   </si>
   <si>
     <t>shreyajaiswal1996vns@gmail.com</t>
+  </si>
+  <si>
+    <t>http://res.cloudinary.com/db5vn6bj5/image/upload/v1635076339/aqod8orn4pcytzivegoe.jpg</t>
+  </si>
+  <si>
+    <t>Deepanshu Gupta</t>
+  </si>
+  <si>
+    <t>tpo@abesit.edu.com</t>
+  </si>
+  <si>
+    <t>jio mart</t>
+  </si>
+  <si>
+    <t>http://res.cloudinary.com/db5vn6bj5/image/upload/v1635076503/bgzcctj8mrxpljmd9a09.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rampur Mumbai </t>
+  </si>
+  <si>
+    <t>Khushabu Belsare</t>
+  </si>
+  <si>
+    <t>khushabubelsare68@gmail.com</t>
+  </si>
+  <si>
+    <t>http://res.cloudinary.com/db5vn6bj5/image/upload/v1635076475/vrzazbmaq5ozrfdnzdsr.jpg</t>
+  </si>
+  <si>
+    <t>kolkata</t>
+  </si>
+  <si>
+    <t>Rahul Tambe</t>
+  </si>
+  <si>
+    <t>iamrahultambe@gmail.com</t>
+  </si>
+  <si>
+    <t>http://res.cloudinary.com/db5vn6bj5/image/upload/v1635076407/hbdxeoukkn7jl8bavygu.jpg</t>
+  </si>
+  <si>
+    <t>Neha Jaiswal</t>
+  </si>
+  <si>
+    <t>nehajaiswal694@gmail.com</t>
+  </si>
+  <si>
+    <t>http://res.cloudinary.com/db5vn6bj5/image/upload/v1635076300/hf4jdrb5p2zh1sgnznuf.jpg</t>
+  </si>
+  <si>
+    <t>MCA</t>
   </si>
 </sst>
 </file>
@@ -457,7 +523,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -550,19 +616,19 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="I3" t="s">
         <v>18</v>
@@ -579,16 +645,16 @@
         <v>1002</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
@@ -607,6 +673,146 @@
       </c>
       <c r="K4">
         <v>9140834289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="1">
+        <v>44493.508656226855</v>
+      </c>
+      <c r="K5">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1004</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="1">
+        <v>44493.508656226855</v>
+      </c>
+      <c r="K6">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1005</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="1">
+        <v>44493.508656226855</v>
+      </c>
+      <c r="K7">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1006</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="1">
+        <v>44493.508656226855</v>
+      </c>
+      <c r="K8">
+        <v>123456789</v>
       </c>
     </row>
   </sheetData>

</xml_diff>